<commit_message>
added test cases for new bugs on the UI
</commit_message>
<xml_diff>
--- a/TestsHome/Test_Cases.xlsx
+++ b/TestsHome/Test_Cases.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOLO CALI\Desktop\FAU FALL 2016\Software Principles\Project\COP4010\TestsHome\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOLO CALI\Desktop\FAU FALL 2016\SoftwarePrinciples\Project\COP4010\TestsHome\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>Test_ID</t>
   </si>
@@ -50,9 +50,6 @@
     <t>User Interface</t>
   </si>
   <si>
-    <t>Color legend</t>
-  </si>
-  <si>
     <t>Usability</t>
   </si>
   <si>
@@ -77,16 +74,148 @@
     <t>COMPATIBILITY</t>
   </si>
   <si>
-    <t>USABILITY</t>
-  </si>
-  <si>
     <t>USER INTERFACE</t>
+  </si>
+  <si>
+    <t>Color coded Permit options on main page</t>
+  </si>
+  <si>
+    <t>color coded parking areas based on occupancy</t>
+  </si>
+  <si>
+    <t>Edge and IE11</t>
+  </si>
+  <si>
+    <t>Welcome animation on welcome page</t>
+  </si>
+  <si>
+    <t>the option to select parking availability based on blue permit</t>
+  </si>
+  <si>
+    <t>the option to select parking availability based on green permit</t>
+  </si>
+  <si>
+    <t>the option to select parking availability based on red permit</t>
+  </si>
+  <si>
+    <t>the option to select parking availability based on parking meter</t>
+  </si>
+  <si>
+    <t>disclaimer message is shown on welcome page</t>
+  </si>
+  <si>
+    <t>disclaimer message is shown on main page</t>
+  </si>
+  <si>
+    <t>general parking rules are shown on main page</t>
+  </si>
+  <si>
+    <t>Color legend is shown in map view page</t>
+  </si>
+  <si>
+    <t>USABILITY/FUNCTIONALITY</t>
+  </si>
+  <si>
+    <t>UI-1</t>
+  </si>
+  <si>
+    <t>UI-2</t>
+  </si>
+  <si>
+    <t>UI-3</t>
+  </si>
+  <si>
+    <t>UI-4</t>
+  </si>
+  <si>
+    <t>UI-5</t>
+  </si>
+  <si>
+    <t>UI-6</t>
+  </si>
+  <si>
+    <t>UI-7</t>
+  </si>
+  <si>
+    <t>UI-8</t>
+  </si>
+  <si>
+    <t>C-1</t>
+  </si>
+  <si>
+    <t>C-2</t>
+  </si>
+  <si>
+    <t>C-3</t>
+  </si>
+  <si>
+    <t>C-4</t>
+  </si>
+  <si>
+    <t>C-5</t>
+  </si>
+  <si>
+    <t>C-6</t>
+  </si>
+  <si>
+    <t>C-7</t>
+  </si>
+  <si>
+    <t>C-8</t>
+  </si>
+  <si>
+    <t>UF-1</t>
+  </si>
+  <si>
+    <t>UF-2</t>
+  </si>
+  <si>
+    <t>UF-3</t>
+  </si>
+  <si>
+    <t>UF-4</t>
+  </si>
+  <si>
+    <t>Bugs/issues</t>
+  </si>
+  <si>
+    <t>Bug1000</t>
+  </si>
+  <si>
+    <t>bug/issue</t>
+  </si>
+  <si>
+    <t>Bug1001</t>
+  </si>
+  <si>
+    <t>Bug1002</t>
+  </si>
+  <si>
+    <t>Bug1003</t>
+  </si>
+  <si>
+    <t>Page 2 - When location drop-down appears, 'Location' button is not centered</t>
+  </si>
+  <si>
+    <t>Page 2 - When location drop-down appears, list is not centered and shrunken down to same size as 'Location' button</t>
+  </si>
+  <si>
+    <t>Page 1 - 'About Us' button does not close when user clicks outside of popup or clicks 'X' contained inside popup (see page 2 for proper functioning)</t>
+  </si>
+  <si>
+    <t>Page 1 - 'Disclaimer' button does not close when user clicks outside of popup or clicks 'X' contained inside popup (see page 2 for proper functioning)</t>
+  </si>
+  <si>
+    <t>UF-5</t>
+  </si>
+  <si>
+    <t>selected item in the Drop-down list updates the correct location</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,13 +292,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -264,6 +394,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -299,6 +446,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,17 +615,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="106.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -485,10 +649,13 @@
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -497,74 +664,282 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>